<commit_message>
still working on modifying data processing script...
</commit_message>
<xml_diff>
--- a/June_Event/Porewaters/pw_raw_npoc_tn_data/20220708_Readme_COMPASS_TEMPEST_JUNE22_n60.xlsx
+++ b/June_Event/Porewaters/pw_raw_npoc_tn_data/20220708_Readme_COMPASS_TEMPEST_JUNE22_n60.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl.sharepoint.com/teams/MCRL-COMPASS/Shared Documents/COMPASS Data Files MCRL/Raw_Instrument_Data/TEMPEST/TOC_LC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myer056/OneDrive - PNNL/Documents/GitHub/TEMPEST/June_Event/Porewaters/pw_raw_npoc_tn_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{7E52ACF1-74BA-FC4F-ABA4-CB04ACC249F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D6C4CE6-5FBD-3341-91B0-C609F62A8F05}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA636FE-A519-884F-B1C1-295F1492391A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="600" windowWidth="14160" windowHeight="15580" activeTab="1" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="28800" windowHeight="16300" xr2:uid="{414E37C4-6C0F-AA42-8BD9-6BC73138264E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Dilution sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>Sample Name</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Total vol (mL)</t>
+  </si>
+  <si>
+    <t>Sample Vol (mL)</t>
   </si>
 </sst>
 </file>
@@ -773,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19AEBD17-6CC0-ED44-B8EB-00F06462890B}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -784,9 +787,11 @@
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -799,8 +804,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -811,7 +822,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -819,7 +830,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -827,7 +838,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -838,7 +849,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -849,7 +860,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -860,7 +871,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -871,7 +882,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -882,7 +893,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -893,7 +904,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -904,7 +915,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -915,7 +926,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -926,7 +937,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -937,7 +948,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -948,7 +959,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1532,22 +1543,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{523C36C3-3BE2-D447-9C28-BD041A6F8A8B}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
@@ -1560,20 +1571,23 @@
       <c r="D1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>102</v>
       </c>
@@ -1586,18 +1600,22 @@
       <c r="D2" s="3">
         <v>0.4703</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
+        <f>D2*0.9998395</f>
+        <v>0.47022451685</v>
+      </c>
+      <c r="F2">
         <v>6.53</v>
       </c>
-      <c r="F2" s="3">
-        <f>D2+E2</f>
+      <c r="G2" s="3">
+        <f>D2+F2</f>
         <v>7.0003000000000002</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>15.7509</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>108</v>
       </c>
@@ -1610,18 +1628,22 @@
       <c r="D3" s="3">
         <v>0.32169999999999999</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E14" si="0">D3*0.9998395</f>
+        <v>0.32164836715</v>
+      </c>
+      <c r="F3">
         <v>6.68</v>
       </c>
-      <c r="F3" s="3">
-        <f t="shared" ref="F3:F14" si="0">D3+E3</f>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G14" si="1">D3+F3</f>
         <v>7.0016999999999996</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>15.600300000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>109</v>
       </c>
@@ -1634,18 +1656,22 @@
       <c r="D4" s="3">
         <v>0.15140000000000001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1513757003</v>
+      </c>
+      <c r="F4">
         <v>6.85</v>
       </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
         <v>7.0013999999999994</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>12.1884</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>111</v>
       </c>
@@ -1658,18 +1684,22 @@
       <c r="D5" s="3">
         <v>3.4643000000000002</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4637439798500003</v>
+      </c>
+      <c r="F5">
         <v>3.5350000000000001</v>
       </c>
-      <c r="F5" s="3">
-        <f t="shared" si="0"/>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
         <v>6.9992999999999999</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>12.228999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>112</v>
       </c>
@@ -1682,18 +1712,22 @@
       <c r="D6" s="3">
         <v>2.9054000000000002</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>2.9049336833000003</v>
+      </c>
+      <c r="F6">
         <v>4.0949999999999998</v>
       </c>
-      <c r="F6" s="3">
-        <f t="shared" si="0"/>
+      <c r="G6" s="3">
+        <f t="shared" si="1"/>
         <v>7.0004</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>15.619300000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>113</v>
       </c>
@@ -1706,18 +1740,22 @@
       <c r="D7" s="3">
         <v>3.2812999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.2807733513499997</v>
+      </c>
+      <c r="F7">
         <v>3.72</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="0"/>
+      <c r="G7" s="3">
+        <f t="shared" si="1"/>
         <v>7.0013000000000005</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>12.198499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>114</v>
       </c>
@@ -1730,18 +1768,22 @@
       <c r="D8" s="3">
         <v>3.6435</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>3.6429152182499998</v>
+      </c>
+      <c r="F8">
         <v>3.355</v>
       </c>
-      <c r="F8" s="3">
-        <f t="shared" si="0"/>
+      <c r="G8" s="3">
+        <f t="shared" si="1"/>
         <v>6.9984999999999999</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>12.106199999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>115</v>
       </c>
@@ -1754,18 +1796,22 @@
       <c r="D9" s="3">
         <v>0.31680000000000003</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3167491536</v>
+      </c>
+      <c r="F9">
         <v>6.6849999999999996</v>
       </c>
-      <c r="F9" s="3">
-        <f t="shared" si="0"/>
+      <c r="G9" s="3">
+        <f t="shared" si="1"/>
         <v>7.0017999999999994</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>15.6387</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>116</v>
       </c>
@@ -1778,18 +1824,22 @@
       <c r="D10" s="3">
         <v>2.3254000000000001</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3250267733000003</v>
+      </c>
+      <c r="F10">
         <v>4.6749999999999998</v>
       </c>
-      <c r="F10" s="3">
-        <f t="shared" si="0"/>
+      <c r="G10" s="3">
+        <f t="shared" si="1"/>
         <v>7.0004</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>12.1625</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>117</v>
       </c>
@@ -1802,18 +1852,22 @@
       <c r="D11" s="3">
         <v>2.8759000000000001</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8754384180499999</v>
+      </c>
+      <c r="F11">
         <v>4.125</v>
       </c>
-      <c r="F11" s="3">
-        <f t="shared" si="0"/>
+      <c r="G11" s="3">
+        <f t="shared" si="1"/>
         <v>7.0008999999999997</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>15.6427</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>118</v>
       </c>
@@ -1826,18 +1880,22 @@
       <c r="D12" s="3">
         <v>2.2284999999999999</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2281423257499999</v>
+      </c>
+      <c r="F12">
         <v>4.915</v>
       </c>
-      <c r="F12" s="3">
-        <f t="shared" si="0"/>
+      <c r="G12" s="3">
+        <f t="shared" si="1"/>
         <v>7.1434999999999995</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>15.7935</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>119</v>
       </c>
@@ -1850,18 +1908,22 @@
       <c r="D13" s="3">
         <v>2.0861999999999998</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.0858651649</v>
+      </c>
+      <c r="F13">
         <v>4.915</v>
       </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
+      <c r="G13" s="3">
+        <f t="shared" si="1"/>
         <v>7.0011999999999999</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>12.0922</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>120</v>
       </c>
@@ -1874,14 +1936,18 @@
       <c r="D14" s="3">
         <v>2.9882</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.9877203939000001</v>
+      </c>
+      <c r="F14">
         <v>4.01</v>
       </c>
-      <c r="F14" s="3">
-        <f t="shared" si="0"/>
+      <c r="G14" s="3">
+        <f t="shared" si="1"/>
         <v>6.9981999999999998</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>15.769500000000001</v>
       </c>
     </row>
@@ -1891,6 +1957,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007324DF9BA5F6B948938C142504C8F34F" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c4aadcd1f2a12dc9b07f6546b5e76248">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="da8c28ad-5ac5-4047-b08a-f75bc24d91a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6457694f174ba676422feeebbff24cf4" ns2:_="">
     <xsd:import namespace="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
@@ -2060,29 +2141,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97452AA2-453B-47A8-B057-FF1E4968504B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FDCC1EA-436B-4072-914B-2C413E47826C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6461AC35-C0A5-49D7-896D-24E61B828141}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6461AC35-C0A5-49D7-896D-24E61B828141}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FDCC1EA-436B-4072-914B-2C413E47826C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97452AA2-453B-47A8-B057-FF1E4968504B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="da8c28ad-5ac5-4047-b08a-f75bc24d91a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>